<commit_message>
Fractura y rigid bodies
</commit_message>
<xml_diff>
--- a/Handbook/PARAMETERS.xlsx
+++ b/Handbook/PARAMETERS.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pedro/REPOs/GM-Dyna/Handbook/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1E09B9D-445C-664E-8520-45A5681A749C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E328C02A-36BF-0849-A79D-5C4D1BF246CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{808B526F-AB2B-2441-8B5B-B133981DB292}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="90">
   <si>
     <t>Number</t>
   </si>
@@ -247,6 +247,54 @@
   </si>
   <si>
     <t>INITIAL DEVIATORIC STRAIN (Es0)</t>
+  </si>
+  <si>
+    <t>Eigenerosion</t>
+  </si>
+  <si>
+    <t>Eigensoftening</t>
+  </si>
+  <si>
+    <t>C EPSILON</t>
+  </si>
+  <si>
+    <t>CEPS</t>
+  </si>
+  <si>
+    <t>WC</t>
+  </si>
+  <si>
+    <t>Wc</t>
+  </si>
+  <si>
+    <t>FT</t>
+  </si>
+  <si>
+    <t>Ft</t>
+  </si>
+  <si>
+    <t>WC_P</t>
+  </si>
+  <si>
+    <t>WC middle point</t>
+  </si>
+  <si>
+    <t>FT_P</t>
+  </si>
+  <si>
+    <t>FT middle point</t>
+  </si>
+  <si>
+    <t>GC</t>
+  </si>
+  <si>
+    <t>Gc</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>Aggregates Size</t>
   </si>
 </sst>
 </file>
@@ -643,11 +691,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C0F23C1-07C1-3B4D-B011-398BF3B62F04}">
-  <dimension ref="B2:J44"/>
+  <dimension ref="B2:L51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E28" sqref="E28:J28"/>
+      <pane ySplit="2" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L52" sqref="L52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -661,10 +709,12 @@
     <col min="7" max="7" width="10.83203125" style="5"/>
     <col min="8" max="8" width="10.83203125" style="4"/>
     <col min="9" max="10" width="10.83203125" style="5"/>
-    <col min="11" max="16384" width="10.83203125" style="4"/>
+    <col min="11" max="11" width="11.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -692,8 +742,14 @@
       <c r="J2" s="3" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="3" spans="2:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K2" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="5">
         <v>1</v>
       </c>
@@ -710,7 +766,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="2:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="5">
         <v>2</v>
       </c>
@@ -727,7 +783,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="2:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="5">
         <v>3</v>
       </c>
@@ -756,7 +812,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="5">
         <v>4</v>
       </c>
@@ -785,7 +841,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="2:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="5">
         <v>5</v>
       </c>
@@ -803,7 +859,7 @@
       </c>
       <c r="H7" s="5"/>
     </row>
-    <row r="8" spans="2:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="5">
         <v>6</v>
       </c>
@@ -821,7 +877,7 @@
       </c>
       <c r="H8" s="5"/>
     </row>
-    <row r="9" spans="2:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="5">
         <v>7</v>
       </c>
@@ -844,7 +900,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="2:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="5">
         <v>8</v>
       </c>
@@ -859,7 +915,7 @@
       </c>
       <c r="H10" s="5"/>
     </row>
-    <row r="11" spans="2:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="5">
         <v>9</v>
       </c>
@@ -874,7 +930,7 @@
       </c>
       <c r="H11" s="5"/>
     </row>
-    <row r="12" spans="2:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="5">
         <v>10</v>
       </c>
@@ -889,7 +945,7 @@
       </c>
       <c r="H12" s="5"/>
     </row>
-    <row r="13" spans="2:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="5">
         <v>11</v>
       </c>
@@ -915,7 +971,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="2:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="5">
         <v>12</v>
       </c>
@@ -936,7 +992,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="2:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="5">
         <v>13</v>
       </c>
@@ -954,7 +1010,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="2:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="5">
         <v>14</v>
       </c>
@@ -1361,7 +1417,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="33" spans="2:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="5">
         <v>31</v>
       </c>
@@ -1375,7 +1431,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="34" spans="2:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="5">
         <v>32</v>
       </c>
@@ -1392,7 +1448,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="35" spans="2:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="5">
         <v>33</v>
       </c>
@@ -1409,7 +1465,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="2:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="5">
         <v>34</v>
       </c>
@@ -1426,7 +1482,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="37" spans="2:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="5">
         <v>35</v>
       </c>
@@ -1443,7 +1499,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="38" spans="2:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="5">
         <v>36</v>
       </c>
@@ -1460,7 +1516,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="39" spans="2:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="5">
         <v>37</v>
       </c>
@@ -1477,7 +1533,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="40" spans="2:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B40" s="5">
         <v>38</v>
       </c>
@@ -1494,7 +1550,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="41" spans="2:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="5">
         <v>39</v>
       </c>
@@ -1511,7 +1567,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="42" spans="2:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B42" s="5">
         <v>40</v>
       </c>
@@ -1528,7 +1584,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="43" spans="2:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B43" s="5">
         <v>41</v>
       </c>
@@ -1545,7 +1601,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="44" spans="2:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B44" s="6">
         <v>42</v>
       </c>
@@ -1571,6 +1627,113 @@
         <v>47</v>
       </c>
       <c r="J44" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="45" spans="2:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B45" s="5">
+        <v>43</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="K45" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="L45" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="46" spans="2:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B46" s="6">
+        <v>44</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="K46" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="L46" s="5"/>
+    </row>
+    <row r="47" spans="2:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B47" s="5">
+        <v>45</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="K47" s="5"/>
+      <c r="L47" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="48" spans="2:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B48" s="6">
+        <v>46</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="K48" s="5"/>
+      <c r="L48" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="2:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B49" s="5">
+        <v>47</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="K49" s="5"/>
+      <c r="L49" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="50" spans="2:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B50" s="6">
+        <v>48</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="K50" s="5"/>
+      <c r="L50" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="51" spans="2:12" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B51" s="5">
+        <v>49</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D51" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="K51" s="5"/>
+      <c r="L51" s="5" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>